<commit_message>
Apache POI login test implemented
</commit_message>
<xml_diff>
--- a/src/main/java/testdataAndDriver/Testdata_Excel.xlsx
+++ b/src/main/java/testdataAndDriver/Testdata_Excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\javaDevelopment\Mobile\appiumWillhabenAndroidappTest\src\main\testdataAndDriver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\javaDevelopment\Mobile\appium-android-native-willhaben\src\main\java\testdataAndDriver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D7B2C7-1972-46DC-B366-4A945D3890FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C18F8F9-60DC-4653-B183-2DBC05630040}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="23040" windowHeight="13898" xr2:uid="{6762633E-1FBB-4206-AE71-0825772920BC}"/>
+    <workbookView xWindow="3043" yWindow="3043" windowWidth="17117" windowHeight="9958" xr2:uid="{6762633E-1FBB-4206-AE71-0825772920BC}"/>
   </bookViews>
   <sheets>
     <sheet name="invalid e-mail format" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <t>excel1@gmx</t>
   </si>
   <si>
-    <t>passwordexcellllllllllllllllllllllllllll</t>
+    <t>passwordexcel</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
parametrized test, README.md, testng.xml, Test_Plan_WiHa.xlsx added
</commit_message>
<xml_diff>
--- a/src/main/java/testdataAndDriver/Testdata_Excel.xlsx
+++ b/src/main/java/testdataAndDriver/Testdata_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\javaDevelopment\Mobile\appium-android-native-willhaben\src\main\java\testdataAndDriver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C18F8F9-60DC-4653-B183-2DBC05630040}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E315178-70D9-4AF3-A300-14318838C829}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3043" yWindow="3043" windowWidth="17117" windowHeight="9958" xr2:uid="{6762633E-1FBB-4206-AE71-0825772920BC}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="23040" windowHeight="13898" xr2:uid="{6762633E-1FBB-4206-AE71-0825772920BC}"/>
   </bookViews>
   <sheets>
     <sheet name="invalid e-mail format" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>E-Mail</t>
   </si>
@@ -33,13 +33,7 @@
     <t>Passwort</t>
   </si>
   <si>
-    <t>invalid email FORMAT in the manual test</t>
-  </si>
-  <si>
     <t>excel1@gmx</t>
-  </si>
-  <si>
-    <t>passwordexcel</t>
   </si>
 </sst>
 </file>
@@ -408,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C33240-0E40-447F-8D9E-BCCC3E2E5D4E}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -420,7 +414,7 @@
     <col min="2" max="2" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,22 +422,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>